<commit_message>
[1159] fix rood sein
</commit_message>
<xml_diff>
--- a/hsl-2022.xlsx
+++ b/hsl-2022.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tom\Code\quickdrive\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1E736CB-C3F1-42DA-863C-49B45E73ED49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55803F89-6057-4A85-8138-E94473DE5F2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="2625" windowWidth="21503" windowHeight="12975" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -69,6 +69,40 @@
 </comments>
 </file>
 
+<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Tom</author>
+  </authors>
+  <commentList>
+    <comment ref="B2" authorId="0" shapeId="0" xr:uid="{17AC6B9E-7850-4A6E-83AF-AD6AD422800D}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Tom:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Rtd4 ipv 6 ivm rood sein</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="65">
   <si>
@@ -283,7 +317,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -311,6 +345,19 @@
       <color indexed="81"/>
       <name val="Tahoma"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="3">
@@ -1554,11 +1601,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CCC9A400-C9E9-4CBA-A9E0-987D9F20D0D9}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CCC9A400-C9E9-4CBA-A9E0-987D9F20D0D9}">
   <dimension ref="A1:B19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1617,9 +1664,11 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A8" s="3"/>
+      <c r="B8" s="4"/>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A9" s="3"/>
+      <c r="B9" s="4"/>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A10" s="3" t="s">
@@ -1683,5 +1732,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
[1159] minor AI fixes
</commit_message>
<xml_diff>
--- a/hsl-2022.xlsx
+++ b/hsl-2022.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tom\Code\quickdrive\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E32359F6-652C-4EFB-811C-8E6E7698BB9A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22A92C03-A6AB-4B90-86F6-A4F784A0FE5F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2625" windowWidth="21503" windowHeight="12975" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-9585" yWindow="2100" windowWidth="21503" windowHeight="12975" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Treinseries" sheetId="1" r:id="rId1"/>
@@ -104,7 +104,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="67">
   <si>
     <t>Treinserie</t>
   </si>
@@ -315,6 +315,9 @@
   <si>
     <t>- Rtd
 - Bd</t>
+  </si>
+  <si>
+    <t>nvt</t>
   </si>
 </sst>
 </file>
@@ -1611,8 +1614,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CCC9A400-C9E9-4CBA-A9E0-987D9F20D0D9}">
   <dimension ref="A1:B19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1728,17 +1731,20 @@
         <v>56</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A17" s="3" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A18" s="3" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="B18" s="4" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A19" s="3" t="s">
         <v>54</v>
       </c>

</xml_diff>